<commit_message>
Modified Excel file and getting data from excel for categories
</commit_message>
<xml_diff>
--- a/src/test/resources/IngredientsAndComorbidities.xlsx
+++ b/src/test/resources/IngredientsAndComorbidities.xlsx
@@ -7,19 +7,20 @@
     <sheet state="visible" name="Final list for LFV Elimination " sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Final list for LCHFElimination " sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="Filter -1 Allergies - Bonus Poi" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Recipe Categories" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataChecksum="v4SQU0p9Lks/GIuIq3hSaF5r68xYc57Vk9JxVhlTvUo="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="8+Qo8DJ85HSzJvPcuxbxe8fgRRaI6dZMfhxS+nidg+k="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="438">
   <si>
     <t>Diabetes</t>
   </si>
@@ -435,7 +436,7 @@
     <t>ghee</t>
   </si>
   <si>
-    <t>microwave meals or ready meals</t>
+    <t>microwave</t>
   </si>
   <si>
     <t>Coffee or tea without sugar</t>
@@ -474,12 +475,18 @@
     <t>sardines</t>
   </si>
   <si>
+    <t>ready meals</t>
+  </si>
+  <si>
     <t>ham</t>
   </si>
   <si>
     <t>cabbage</t>
   </si>
   <si>
+    <t>processed</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -669,13 +676,13 @@
     <t>tangerine</t>
   </si>
   <si>
-    <t>all berry varieties</t>
+    <t>berry</t>
   </si>
   <si>
     <t>pastry</t>
   </si>
   <si>
-    <t>all melon varieties</t>
+    <t>melon</t>
   </si>
   <si>
     <t>cakes</t>
@@ -879,7 +886,7 @@
     <t>stevia</t>
   </si>
   <si>
-    <t>all forms of chana</t>
+    <t>chana</t>
   </si>
   <si>
     <t>barley malt</t>
@@ -888,6 +895,9 @@
     <t>almond</t>
   </si>
   <si>
+    <t>curd</t>
+  </si>
+  <si>
     <t>cashew</t>
   </si>
   <si>
@@ -939,7 +949,7 @@
     <t>Ham</t>
   </si>
   <si>
-    <t>Processed Foods</t>
+    <t>Processed</t>
   </si>
   <si>
     <t>1.       Raw,</t>
@@ -1047,9 +1057,6 @@
     <t>condensed milk</t>
   </si>
   <si>
-    <t>curd</t>
-  </si>
-  <si>
     <t>sunflower seed</t>
   </si>
   <si>
@@ -1132,13 +1139,208 @@
   </si>
   <si>
     <t>Seafood</t>
+  </si>
+  <si>
+    <t>Recipe Tag Categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foodcategory                          </t>
+  </si>
+  <si>
+    <t>cuisinecategory</t>
+  </si>
+  <si>
+    <t>recipecategory</t>
+  </si>
+  <si>
+    <t>subcategory</t>
+  </si>
+  <si>
+    <t>foodprocessing</t>
+  </si>
+  <si>
+    <t>foodprocessingtoavoid</t>
+  </si>
+  <si>
+    <t>Vegan</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
+    <t>Roti</t>
+  </si>
+  <si>
+    <t>Raw</t>
+  </si>
+  <si>
+    <t>Microwave</t>
+  </si>
+  <si>
+    <t>Vegetarian</t>
+  </si>
+  <si>
+    <t>South Indian</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Soup</t>
+  </si>
+  <si>
+    <t>Steamed</t>
+  </si>
+  <si>
+    <t>Jain</t>
+  </si>
+  <si>
+    <t>Rajasthani</t>
+  </si>
+  <si>
+    <t>Snack</t>
+  </si>
+  <si>
+    <t>Salad</t>
+  </si>
+  <si>
+    <t>Boiled</t>
+  </si>
+  <si>
+    <t>Fried</t>
+  </si>
+  <si>
+    <t>Eggitarian</t>
+  </si>
+  <si>
+    <t>Punjabi</t>
+  </si>
+  <si>
+    <t>Dinner</t>
+  </si>
+  <si>
+    <t>Starter</t>
+  </si>
+  <si>
+    <t>porched</t>
+  </si>
+  <si>
+    <t>Non-veg</t>
+  </si>
+  <si>
+    <t>Bengali</t>
+  </si>
+  <si>
+    <t>Drink</t>
+  </si>
+  <si>
+    <t>sauted</t>
+  </si>
+  <si>
+    <t>Crackers</t>
+  </si>
+  <si>
+    <t>orissa</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Airfryed</t>
+  </si>
+  <si>
+    <t>Gujarati</t>
+  </si>
+  <si>
+    <t>Noodles</t>
+  </si>
+  <si>
+    <t>panfryed</t>
+  </si>
+  <si>
+    <t>Maharashtrian</t>
+  </si>
+  <si>
+    <t>Curry</t>
+  </si>
+  <si>
+    <t>Andhra</t>
+  </si>
+  <si>
+    <t>Kerala</t>
+  </si>
+  <si>
+    <t>Goan</t>
+  </si>
+  <si>
+    <t>Kashmiri</t>
+  </si>
+  <si>
+    <t>Himachali</t>
+  </si>
+  <si>
+    <t>Tamil nadu</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>Sindhi</t>
+  </si>
+  <si>
+    <t>Chhattisgarhi</t>
+  </si>
+  <si>
+    <t>Madhya pradesh</t>
+  </si>
+  <si>
+    <t>Assamese</t>
+  </si>
+  <si>
+    <t>Manipuri</t>
+  </si>
+  <si>
+    <t>Tripuri</t>
+  </si>
+  <si>
+    <t>Sikkimese</t>
+  </si>
+  <si>
+    <t>Mizo</t>
+  </si>
+  <si>
+    <t>Arunachali</t>
+  </si>
+  <si>
+    <t>uttarakhand</t>
+  </si>
+  <si>
+    <t>Haryanvi</t>
+  </si>
+  <si>
+    <t>Awadhi</t>
+  </si>
+  <si>
+    <t>Bihari</t>
+  </si>
+  <si>
+    <t>Uttar pradesh</t>
+  </si>
+  <si>
+    <t>Delhi</t>
+  </si>
+  <si>
+    <t>North Indian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1167,29 +1369,29 @@
       <sz val="28.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="14.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <color rgb="FF212B32"/>
-      <name val="&quot;Frutiger W01&quot;"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF212B32"/>
+      <name val="&quot;Frutiger W01&quot;"/>
     </font>
     <font>
       <b/>
@@ -1201,6 +1403,10 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
       <color theme="1"/>
@@ -1233,7 +1439,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border/>
     <border>
       <left style="thin">
@@ -1402,11 +1608,30 @@
         <color rgb="FFA5A5A5"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1463,35 +1688,60 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="12" fillId="4" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="12" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="12" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="13" fillId="2" fontId="12" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="13" fillId="2" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="14" fillId="2" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="15" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="15" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="15" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="14" fillId="2" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="14" fillId="2" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1515,6 +1765,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -30140,7 +30394,7 @@
       <c r="D5" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="22"/>
     </row>
     <row r="6">
       <c r="A6" s="22" t="s">
@@ -30155,7 +30409,7 @@
       <c r="D6" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="22"/>
     </row>
     <row r="7">
       <c r="A7" s="22" t="s">
@@ -30167,899 +30421,905 @@
       <c r="C7" s="22" t="s">
         <v>150</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="E7" s="22"/>
     </row>
     <row r="8">
       <c r="A8" s="22" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+        <v>153</v>
+      </c>
+      <c r="C8" s="22"/>
+      <c r="D8" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="22"/>
       <c r="H8" s="25" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+        <v>157</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
     </row>
     <row r="10">
       <c r="A10" s="22" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C10" s="27"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
     </row>
     <row r="11">
       <c r="A11" s="22" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>159</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+        <v>161</v>
+      </c>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
     </row>
     <row r="12">
       <c r="A12" s="22" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
+        <v>163</v>
+      </c>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13">
       <c r="A13" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
+        <v>165</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
     </row>
     <row r="14">
       <c r="A14" s="22" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
+        <v>167</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
     </row>
     <row r="15">
       <c r="A15" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
+        <v>169</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16">
       <c r="A16" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
+        <v>171</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
     </row>
     <row r="17">
       <c r="A17" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
+        <v>173</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
     </row>
     <row r="18">
       <c r="A18" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
+        <v>175</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
       <c r="J18" s="25" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="22" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
+        <v>178</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
     </row>
     <row r="20">
       <c r="A20" s="22" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
+        <v>180</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
     </row>
     <row r="21">
       <c r="A21" s="22" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
+        <v>182</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
     </row>
     <row r="22">
       <c r="A22" s="22" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
+        <v>184</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
     </row>
     <row r="23">
       <c r="A23" s="22" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
+        <v>186</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
     </row>
     <row r="24">
       <c r="A24" s="22" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
+        <v>175</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
     </row>
     <row r="25">
       <c r="A25" s="22" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
+        <v>189</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
     </row>
     <row r="26">
       <c r="A26" s="22" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
+        <v>191</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
     </row>
     <row r="27">
       <c r="A27" s="22" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
+        <v>193</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
     </row>
     <row r="28">
       <c r="A28" s="22" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
+        <v>195</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
     </row>
     <row r="29">
       <c r="A29" s="22" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
+        <v>197</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
     </row>
     <row r="30">
       <c r="A30" s="22" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
+        <v>199</v>
+      </c>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
     </row>
     <row r="31">
       <c r="A31" s="22" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
+        <v>201</v>
+      </c>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32">
       <c r="A32" s="22" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
+        <v>203</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
     </row>
     <row r="33">
       <c r="A33" s="22" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
+        <v>205</v>
+      </c>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
     </row>
     <row r="34">
       <c r="A34" s="22" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
+        <v>207</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
     </row>
     <row r="35">
       <c r="A35" s="22" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
+        <v>209</v>
+      </c>
+      <c r="C35" s="28"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
     </row>
     <row r="36">
       <c r="A36" s="22" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
+        <v>211</v>
+      </c>
+      <c r="C36" s="28"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
     </row>
     <row r="37">
       <c r="A37" s="22" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
+        <v>213</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
     </row>
     <row r="38">
       <c r="A38" s="22" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="C38" s="23"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
+        <v>215</v>
+      </c>
+      <c r="C38" s="28"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
     </row>
     <row r="39">
       <c r="A39" s="22" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
+        <v>217</v>
+      </c>
+      <c r="C39" s="28"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
     </row>
     <row r="40">
       <c r="A40" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
+      <c r="B40" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="C40" s="28"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
     </row>
     <row r="41">
       <c r="A41" s="22" t="s">
-        <v>217</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
+        <v>219</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
     </row>
     <row r="42">
       <c r="A42" s="22" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
+        <v>222</v>
+      </c>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="22"/>
     </row>
     <row r="43">
       <c r="A43" s="22" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C43" s="27"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
+      <c r="D43" s="22"/>
+      <c r="E43" s="22"/>
     </row>
     <row r="44">
       <c r="A44" s="22" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
+        <v>226</v>
+      </c>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
     </row>
     <row r="45">
       <c r="A45" s="22" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
+        <v>228</v>
+      </c>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="22"/>
     </row>
     <row r="46">
       <c r="A46" s="22" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C46" s="27"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="22"/>
     </row>
     <row r="47">
       <c r="A47" s="22" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
+        <v>232</v>
+      </c>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
     </row>
     <row r="48">
       <c r="A48" s="22" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
+        <v>234</v>
+      </c>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
     </row>
     <row r="49">
       <c r="A49" s="22" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>234</v>
-      </c>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
+        <v>236</v>
+      </c>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
+      <c r="E49" s="22"/>
     </row>
     <row r="50">
       <c r="A50" s="22" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
+        <v>238</v>
+      </c>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
     </row>
     <row r="51">
       <c r="A51" s="22" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
+        <v>240</v>
+      </c>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
     </row>
     <row r="52">
       <c r="A52" s="22" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
+        <v>242</v>
+      </c>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
     </row>
     <row r="53">
       <c r="A53" s="22" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>242</v>
-      </c>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
+        <v>244</v>
+      </c>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
     </row>
     <row r="54">
       <c r="A54" s="22" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>244</v>
-      </c>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
+        <v>246</v>
+      </c>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
     </row>
     <row r="55">
       <c r="A55" s="22" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
+        <v>248</v>
+      </c>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
+      <c r="E55" s="22"/>
     </row>
     <row r="56">
       <c r="A56" s="22" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
+        <v>250</v>
+      </c>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
     </row>
     <row r="57">
       <c r="A57" s="22" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>250</v>
-      </c>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
+        <v>252</v>
+      </c>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
     </row>
     <row r="58">
       <c r="A58" s="22" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>252</v>
-      </c>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
-      <c r="E58" s="24"/>
+        <v>254</v>
+      </c>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
     </row>
     <row r="59">
       <c r="A59" s="22" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>254</v>
-      </c>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24"/>
+        <v>256</v>
+      </c>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="22"/>
     </row>
     <row r="60">
       <c r="A60" s="22" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>256</v>
-      </c>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
+        <v>258</v>
+      </c>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
+      <c r="E60" s="22"/>
     </row>
     <row r="61">
       <c r="A61" s="22" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>258</v>
-      </c>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
-      <c r="E61" s="24"/>
+        <v>260</v>
+      </c>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
+      <c r="E61" s="22"/>
     </row>
     <row r="62">
       <c r="A62" s="22" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>260</v>
-      </c>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
+        <v>262</v>
+      </c>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="22"/>
     </row>
     <row r="63">
       <c r="A63" s="22" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>262</v>
-      </c>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
-      <c r="E63" s="24"/>
+        <v>264</v>
+      </c>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="22"/>
     </row>
     <row r="64">
       <c r="A64" s="22" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
+        <v>266</v>
+      </c>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="22"/>
     </row>
     <row r="65">
       <c r="A65" s="22" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>266</v>
-      </c>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
+        <v>268</v>
+      </c>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="22"/>
     </row>
     <row r="66">
       <c r="A66" s="22" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>268</v>
-      </c>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
+        <v>270</v>
+      </c>
+      <c r="C66" s="22"/>
+      <c r="D66" s="22"/>
+      <c r="E66" s="22"/>
     </row>
     <row r="67">
       <c r="A67" s="22" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>270</v>
-      </c>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
+        <v>272</v>
+      </c>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
+      <c r="E67" s="22"/>
     </row>
     <row r="68">
       <c r="A68" s="22" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>272</v>
-      </c>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
+        <v>274</v>
+      </c>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="22"/>
     </row>
     <row r="69">
       <c r="A69" s="22" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>274</v>
-      </c>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
+        <v>276</v>
+      </c>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
     </row>
     <row r="70">
       <c r="A70" s="22" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>276</v>
-      </c>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
+        <v>278</v>
+      </c>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
     </row>
     <row r="71">
       <c r="A71" s="22" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>278</v>
-      </c>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
+        <v>280</v>
+      </c>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
     </row>
     <row r="72">
       <c r="A72" s="22" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="C72" s="24"/>
-      <c r="D72" s="24"/>
-      <c r="E72" s="24"/>
+        <v>282</v>
+      </c>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
+      <c r="E72" s="22"/>
     </row>
     <row r="73">
       <c r="A73" s="22" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
+        <v>284</v>
+      </c>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
+      <c r="E73" s="22"/>
     </row>
     <row r="74">
       <c r="A74" s="22" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>284</v>
-      </c>
-      <c r="C74" s="24"/>
-      <c r="D74" s="24"/>
-      <c r="E74" s="24"/>
+        <v>286</v>
+      </c>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
     </row>
     <row r="75">
       <c r="A75" s="22" t="s">
-        <v>285</v>
-      </c>
-      <c r="B75" s="22" t="s">
-        <v>286</v>
-      </c>
-      <c r="C75" s="24"/>
-      <c r="D75" s="24"/>
-      <c r="E75" s="24"/>
+        <v>287</v>
+      </c>
+      <c r="B75" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
+      <c r="E75" s="22"/>
     </row>
     <row r="76">
       <c r="A76" s="22" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>288</v>
-      </c>
-      <c r="C76" s="24"/>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
+        <v>290</v>
+      </c>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="22"/>
     </row>
     <row r="77">
-      <c r="A77" s="24"/>
+      <c r="A77" s="24" t="s">
+        <v>291</v>
+      </c>
       <c r="B77" s="22" t="s">
-        <v>289</v>
-      </c>
-      <c r="C77" s="24"/>
-      <c r="D77" s="24"/>
-      <c r="E77" s="24"/>
+        <v>292</v>
+      </c>
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="22"/>
     </row>
     <row r="78">
-      <c r="A78" s="24"/>
+      <c r="A78" s="22"/>
       <c r="B78" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
+        <v>293</v>
+      </c>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
     </row>
     <row r="79">
-      <c r="A79" s="24"/>
+      <c r="A79" s="22"/>
       <c r="B79" s="22" t="s">
-        <v>291</v>
-      </c>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
+        <v>294</v>
+      </c>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="22"/>
     </row>
     <row r="80">
-      <c r="A80" s="24"/>
+      <c r="A80" s="22"/>
       <c r="B80" s="22" t="s">
-        <v>292</v>
-      </c>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="24"/>
+        <v>295</v>
+      </c>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
     </row>
     <row r="81">
-      <c r="A81" s="24"/>
+      <c r="A81" s="22"/>
       <c r="B81" s="22" t="s">
-        <v>293</v>
-      </c>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
+        <v>296</v>
+      </c>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
     </row>
     <row r="82">
-      <c r="A82" s="24"/>
+      <c r="A82" s="22"/>
       <c r="B82" s="22" t="s">
-        <v>294</v>
-      </c>
-      <c r="C82" s="24"/>
-      <c r="D82" s="24"/>
-      <c r="E82" s="24"/>
+        <v>297</v>
+      </c>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
+      <c r="E82" s="22"/>
     </row>
     <row r="83">
-      <c r="A83" s="24"/>
+      <c r="A83" s="22"/>
       <c r="B83" s="22" t="s">
-        <v>295</v>
-      </c>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
-      <c r="E83" s="24"/>
+        <v>298</v>
+      </c>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="22"/>
     </row>
     <row r="84">
-      <c r="A84" s="24"/>
+      <c r="A84" s="22"/>
       <c r="B84" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
+        <v>299</v>
+      </c>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
+      <c r="E84" s="22"/>
     </row>
     <row r="85">
-      <c r="A85" s="24"/>
+      <c r="A85" s="22"/>
       <c r="B85" s="22" t="s">
-        <v>297</v>
-      </c>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
+        <v>300</v>
+      </c>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
     </row>
     <row r="86">
-      <c r="A86" s="24"/>
+      <c r="A86" s="22"/>
       <c r="B86" s="22" t="s">
-        <v>298</v>
-      </c>
-      <c r="C86" s="24"/>
-      <c r="D86" s="24"/>
-      <c r="E86" s="24"/>
+        <v>301</v>
+      </c>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
     </row>
     <row r="87">
-      <c r="A87" s="24"/>
+      <c r="A87" s="22"/>
       <c r="B87" s="22" t="s">
-        <v>299</v>
-      </c>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
+        <v>302</v>
+      </c>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
+      <c r="E87" s="22"/>
     </row>
     <row r="88">
-      <c r="A88" s="24"/>
+      <c r="A88" s="22"/>
       <c r="B88" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="C88" s="24"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
+        <v>303</v>
+      </c>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
+      <c r="E88" s="22"/>
     </row>
     <row r="89">
-      <c r="A89" s="24"/>
+      <c r="A89" s="22"/>
       <c r="B89" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
-      <c r="E89" s="24"/>
+        <v>304</v>
+      </c>
+      <c r="C89" s="22"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="22"/>
     </row>
     <row r="90">
-      <c r="A90" s="24"/>
+      <c r="A90" s="22"/>
       <c r="B90" s="22" t="s">
-        <v>302</v>
-      </c>
-      <c r="C90" s="24"/>
-      <c r="D90" s="24"/>
-      <c r="E90" s="24"/>
+        <v>305</v>
+      </c>
+      <c r="C90" s="22"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -31087,7 +31347,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -31104,57 +31364,57 @@
         <v>128</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="22" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="B3" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>306</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>307</v>
+      <c r="C3" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="22" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="29" t="s">
-        <v>309</v>
+        <v>172</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="30" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="22" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>311</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="29" t="s">
-        <v>312</v>
+        <v>314</v>
+      </c>
+      <c r="C5" s="22"/>
+      <c r="D5" s="30" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="22" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="29" t="s">
-        <v>314</v>
+        <v>170</v>
+      </c>
+      <c r="C6" s="22"/>
+      <c r="D6" s="30" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="7">
@@ -31162,756 +31422,756 @@
         <v>150</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>315</v>
-      </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="29" t="s">
-        <v>316</v>
+        <v>318</v>
+      </c>
+      <c r="C7" s="22"/>
+      <c r="D7" s="30" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="22" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B8" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="29" t="s">
-        <v>317</v>
+      <c r="C8" s="22"/>
+      <c r="D8" s="30" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="22" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>319</v>
-      </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="29" t="s">
-        <v>320</v>
+        <v>322</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="30" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>321</v>
-      </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
+        <v>324</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
     </row>
     <row r="11">
       <c r="A11" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B11" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
     </row>
     <row r="12">
       <c r="A12" s="22" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
     </row>
     <row r="13">
       <c r="A13" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>323</v>
-      </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
+        <v>326</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
     </row>
     <row r="14">
       <c r="A14" s="22" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>325</v>
-      </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+        <v>328</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
     </row>
     <row r="15">
       <c r="A15" s="22" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>327</v>
-      </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
+        <v>330</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
     </row>
     <row r="16">
       <c r="A16" s="22" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>329</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
+        <v>332</v>
+      </c>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
     </row>
     <row r="17">
       <c r="A17" s="22" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>331</v>
-      </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
+        <v>334</v>
+      </c>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
     </row>
     <row r="18">
       <c r="A18" s="22" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>333</v>
-      </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
+        <v>336</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
     </row>
     <row r="19">
       <c r="A19" s="22" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>288</v>
-      </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
+        <v>290</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
     </row>
     <row r="20">
       <c r="A20" s="22" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
+        <v>293</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
     </row>
     <row r="21">
       <c r="A21" s="22" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>291</v>
-      </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
+        <v>294</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
     </row>
     <row r="22">
       <c r="A22" s="22" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>292</v>
-      </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
+        <v>295</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
     </row>
     <row r="23">
       <c r="A23" s="22" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>293</v>
-      </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
+        <v>296</v>
+      </c>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
     </row>
     <row r="24">
       <c r="A24" s="22" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>294</v>
-      </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
+        <v>297</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
     </row>
     <row r="25">
       <c r="A25" s="22" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>295</v>
-      </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
+        <v>298</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
     </row>
     <row r="26">
       <c r="A26" s="22" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
+        <v>299</v>
+      </c>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
     </row>
     <row r="27">
       <c r="A27" s="22" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>298</v>
-      </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
+        <v>301</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
     </row>
     <row r="28">
       <c r="A28" s="22" t="s">
-        <v>342</v>
+        <v>291</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>343</v>
-      </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
+        <v>345</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
     </row>
     <row r="29">
       <c r="A29" s="22" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
+        <v>303</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
     </row>
     <row r="30">
       <c r="A30" s="22" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
+        <v>304</v>
+      </c>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
     </row>
     <row r="31">
       <c r="A31" s="22" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>302</v>
-      </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
+        <v>305</v>
+      </c>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
     </row>
     <row r="32">
       <c r="A32" s="22" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>348</v>
-      </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
+        <v>350</v>
+      </c>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
     </row>
     <row r="33">
       <c r="A33" s="22" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>350</v>
-      </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
+        <v>352</v>
+      </c>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
     </row>
     <row r="34">
       <c r="A34" s="22" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>352</v>
-      </c>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
+        <v>354</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
     </row>
     <row r="35">
       <c r="A35" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
+        <v>355</v>
+      </c>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
     </row>
     <row r="36">
       <c r="A36" s="22" t="s">
-        <v>354</v>
-      </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
+        <v>356</v>
+      </c>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
     </row>
     <row r="37">
       <c r="A37" s="22" t="s">
-        <v>355</v>
-      </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
+        <v>357</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
     </row>
     <row r="38">
       <c r="A38" s="22" t="s">
-        <v>356</v>
-      </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
+        <v>358</v>
+      </c>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
     </row>
     <row r="39">
       <c r="A39" s="22" t="s">
-        <v>357</v>
-      </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
+        <v>359</v>
+      </c>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
     </row>
     <row r="40">
       <c r="A40" s="22" t="s">
-        <v>266</v>
-      </c>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
+        <v>268</v>
+      </c>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
     </row>
     <row r="41">
       <c r="A41" s="22" t="s">
-        <v>260</v>
-      </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
+        <v>262</v>
+      </c>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
     </row>
     <row r="42">
       <c r="A42" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
+        <v>360</v>
+      </c>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
     </row>
     <row r="43">
       <c r="A43" s="22" t="s">
-        <v>359</v>
-      </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
+        <v>361</v>
+      </c>
+      <c r="B43" s="22"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="22"/>
     </row>
     <row r="44">
       <c r="A44" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
+        <v>362</v>
+      </c>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
     </row>
     <row r="45">
       <c r="A45" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
+        <v>201</v>
+      </c>
+      <c r="B45" s="22"/>
+      <c r="C45" s="22"/>
+      <c r="D45" s="22"/>
     </row>
     <row r="46">
       <c r="A46" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
+        <v>203</v>
+      </c>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
     </row>
     <row r="47">
       <c r="A47" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
+        <v>205</v>
+      </c>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
     </row>
     <row r="48">
       <c r="A48" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
+        <v>207</v>
+      </c>
+      <c r="B48" s="22"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
     </row>
     <row r="49">
       <c r="A49" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
+        <v>209</v>
+      </c>
+      <c r="B49" s="22"/>
+      <c r="C49" s="22"/>
+      <c r="D49" s="22"/>
     </row>
     <row r="50">
       <c r="A50" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="24"/>
+        <v>211</v>
+      </c>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
     </row>
     <row r="51">
       <c r="A51" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
+        <v>213</v>
+      </c>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
     </row>
     <row r="52">
       <c r="A52" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
+        <v>215</v>
+      </c>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22"/>
+      <c r="D52" s="22"/>
     </row>
     <row r="53">
       <c r="A53" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
+        <v>217</v>
+      </c>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22"/>
+      <c r="D53" s="22"/>
     </row>
     <row r="54">
-      <c r="A54" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
+      <c r="A54" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
     </row>
     <row r="55">
       <c r="A55" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
+        <v>222</v>
+      </c>
+      <c r="B55" s="22"/>
+      <c r="C55" s="22"/>
+      <c r="D55" s="22"/>
     </row>
     <row r="56">
       <c r="A56" s="22" t="s">
-        <v>222</v>
-      </c>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24"/>
-      <c r="D56" s="24"/>
+        <v>224</v>
+      </c>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
     </row>
     <row r="57">
       <c r="A57" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
+        <v>226</v>
+      </c>
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
     </row>
     <row r="58">
       <c r="A58" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="B58" s="24"/>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
+        <v>228</v>
+      </c>
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
     </row>
     <row r="59">
       <c r="A59" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
+        <v>177</v>
+      </c>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
     </row>
     <row r="60">
       <c r="A60" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
+        <v>179</v>
+      </c>
+      <c r="B60" s="22"/>
+      <c r="C60" s="22"/>
+      <c r="D60" s="22"/>
     </row>
     <row r="61">
       <c r="A61" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="B61" s="24"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
+        <v>181</v>
+      </c>
+      <c r="B61" s="22"/>
+      <c r="C61" s="22"/>
+      <c r="D61" s="22"/>
     </row>
     <row r="62">
       <c r="A62" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
+        <v>183</v>
+      </c>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
     </row>
     <row r="63">
       <c r="A63" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="B63" s="24"/>
-      <c r="C63" s="24"/>
-      <c r="D63" s="24"/>
+        <v>185</v>
+      </c>
+      <c r="B63" s="22"/>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
     </row>
     <row r="64">
       <c r="A64" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="B64" s="24"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
+        <v>187</v>
+      </c>
+      <c r="B64" s="22"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
     </row>
     <row r="65">
       <c r="A65" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B65" s="24"/>
-      <c r="C65" s="24"/>
-      <c r="D65" s="24"/>
+        <v>188</v>
+      </c>
+      <c r="B65" s="22"/>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
     </row>
     <row r="66">
       <c r="A66" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="B66" s="24"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
+        <v>190</v>
+      </c>
+      <c r="B66" s="22"/>
+      <c r="C66" s="22"/>
+      <c r="D66" s="22"/>
     </row>
     <row r="67">
       <c r="A67" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
+        <v>192</v>
+      </c>
+      <c r="B67" s="22"/>
+      <c r="C67" s="22"/>
+      <c r="D67" s="22"/>
     </row>
     <row r="68">
       <c r="A68" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
+        <v>194</v>
+      </c>
+      <c r="B68" s="22"/>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
     </row>
     <row r="69">
       <c r="A69" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="B69" s="24"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
+        <v>196</v>
+      </c>
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="22"/>
     </row>
     <row r="70">
       <c r="A70" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="B70" s="24"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
+        <v>251</v>
+      </c>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
     </row>
     <row r="71">
       <c r="A71" s="22" t="s">
-        <v>251</v>
-      </c>
-      <c r="B71" s="24"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
+        <v>253</v>
+      </c>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
     </row>
     <row r="72">
       <c r="A72" s="22" t="s">
-        <v>253</v>
-      </c>
-      <c r="B72" s="24"/>
-      <c r="C72" s="24"/>
-      <c r="D72" s="24"/>
+        <v>255</v>
+      </c>
+      <c r="B72" s="22"/>
+      <c r="C72" s="22"/>
+      <c r="D72" s="22"/>
     </row>
     <row r="73">
       <c r="A73" s="22" t="s">
-        <v>255</v>
-      </c>
-      <c r="B73" s="24"/>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
+        <v>257</v>
+      </c>
+      <c r="B73" s="22"/>
+      <c r="C73" s="22"/>
+      <c r="D73" s="22"/>
     </row>
     <row r="74">
       <c r="A74" s="22" t="s">
-        <v>257</v>
-      </c>
-      <c r="B74" s="24"/>
-      <c r="C74" s="24"/>
-      <c r="D74" s="24"/>
+        <v>259</v>
+      </c>
+      <c r="B74" s="22"/>
+      <c r="C74" s="22"/>
+      <c r="D74" s="22"/>
     </row>
     <row r="75">
       <c r="A75" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="24"/>
+        <v>261</v>
+      </c>
+      <c r="B75" s="22"/>
+      <c r="C75" s="22"/>
+      <c r="D75" s="22"/>
     </row>
     <row r="76">
       <c r="A76" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="B76" s="24"/>
-      <c r="C76" s="24"/>
-      <c r="D76" s="24"/>
+        <v>263</v>
+      </c>
+      <c r="B76" s="22"/>
+      <c r="C76" s="22"/>
+      <c r="D76" s="22"/>
     </row>
     <row r="77">
       <c r="A77" s="22" t="s">
-        <v>361</v>
-      </c>
-      <c r="B77" s="24"/>
-      <c r="C77" s="24"/>
-      <c r="D77" s="24"/>
+        <v>363</v>
+      </c>
+      <c r="B77" s="22"/>
+      <c r="C77" s="22"/>
+      <c r="D77" s="22"/>
     </row>
     <row r="78">
       <c r="A78" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="B78" s="24"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
+        <v>267</v>
+      </c>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+      <c r="D78" s="22"/>
     </row>
     <row r="79">
       <c r="A79" s="22" t="s">
-        <v>267</v>
-      </c>
-      <c r="B79" s="24"/>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
+        <v>269</v>
+      </c>
+      <c r="B79" s="22"/>
+      <c r="C79" s="22"/>
+      <c r="D79" s="22"/>
     </row>
     <row r="80">
       <c r="A80" s="22" t="s">
-        <v>269</v>
-      </c>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
+        <v>271</v>
+      </c>
+      <c r="B80" s="22"/>
+      <c r="C80" s="22"/>
+      <c r="D80" s="22"/>
     </row>
     <row r="81">
       <c r="A81" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
+        <v>273</v>
+      </c>
+      <c r="B81" s="22"/>
+      <c r="C81" s="22"/>
+      <c r="D81" s="22"/>
     </row>
     <row r="82">
       <c r="A82" s="22" t="s">
-        <v>273</v>
-      </c>
-      <c r="B82" s="24"/>
-      <c r="C82" s="24"/>
-      <c r="D82" s="24"/>
+        <v>275</v>
+      </c>
+      <c r="B82" s="22"/>
+      <c r="C82" s="22"/>
+      <c r="D82" s="22"/>
     </row>
     <row r="83">
       <c r="A83" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="B83" s="24"/>
-      <c r="C83" s="24"/>
-      <c r="D83" s="24"/>
+        <v>277</v>
+      </c>
+      <c r="B83" s="22"/>
+      <c r="C83" s="22"/>
+      <c r="D83" s="22"/>
     </row>
     <row r="84">
       <c r="A84" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
-      <c r="D84" s="24"/>
+        <v>279</v>
+      </c>
+      <c r="B84" s="22"/>
+      <c r="C84" s="22"/>
+      <c r="D84" s="22"/>
     </row>
     <row r="85">
       <c r="A85" s="22" t="s">
-        <v>279</v>
-      </c>
-      <c r="B85" s="24"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
+        <v>281</v>
+      </c>
+      <c r="B85" s="22"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
     </row>
     <row r="86">
       <c r="A86" s="22" t="s">
-        <v>281</v>
-      </c>
-      <c r="B86" s="24"/>
-      <c r="C86" s="24"/>
-      <c r="D86" s="24"/>
+        <v>283</v>
+      </c>
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+      <c r="D86" s="22"/>
     </row>
     <row r="87">
       <c r="A87" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="B87" s="24"/>
-      <c r="C87" s="24"/>
-      <c r="D87" s="24"/>
+        <v>285</v>
+      </c>
+      <c r="B87" s="22"/>
+      <c r="C87" s="22"/>
+      <c r="D87" s="22"/>
     </row>
     <row r="88">
       <c r="A88" s="22" t="s">
-        <v>285</v>
-      </c>
-      <c r="B88" s="24"/>
-      <c r="C88" s="24"/>
-      <c r="D88" s="24"/>
+        <v>287</v>
+      </c>
+      <c r="B88" s="22"/>
+      <c r="C88" s="22"/>
+      <c r="D88" s="22"/>
     </row>
     <row r="89">
       <c r="A89" s="22" t="s">
-        <v>287</v>
-      </c>
-      <c r="B89" s="24"/>
-      <c r="C89" s="24"/>
-      <c r="D89" s="24"/>
+        <v>289</v>
+      </c>
+      <c r="B89" s="22"/>
+      <c r="C89" s="22"/>
+      <c r="D89" s="22"/>
     </row>
     <row r="90">
       <c r="A90" s="22" t="s">
-        <v>362</v>
-      </c>
-      <c r="B90" s="24"/>
-      <c r="C90" s="24"/>
-      <c r="D90" s="24"/>
+        <v>364</v>
+      </c>
+      <c r="B90" s="22"/>
+      <c r="C90" s="22"/>
+      <c r="D90" s="22"/>
     </row>
     <row r="91">
       <c r="A91" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="B91" s="24"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
+        <v>360</v>
+      </c>
+      <c r="B91" s="22"/>
+      <c r="C91" s="22"/>
+      <c r="D91" s="22"/>
     </row>
     <row r="92">
       <c r="A92" s="22" t="s">
-        <v>363</v>
-      </c>
-      <c r="B92" s="24"/>
-      <c r="C92" s="24"/>
-      <c r="D92" s="24"/>
+        <v>365</v>
+      </c>
+      <c r="B92" s="22"/>
+      <c r="C92" s="22"/>
+      <c r="D92" s="22"/>
     </row>
     <row r="93">
-      <c r="A93" s="24"/>
-      <c r="B93" s="24"/>
-      <c r="C93" s="24"/>
-      <c r="D93" s="24"/>
+      <c r="A93" s="22"/>
+      <c r="B93" s="22"/>
+      <c r="C93" s="22"/>
+      <c r="D93" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -31936,75 +32196,501 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="21" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="30" t="s">
-        <v>365</v>
+      <c r="A2" s="31" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="30" t="s">
-        <v>366</v>
+      <c r="A3" s="31" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="30" t="s">
-        <v>367</v>
+      <c r="A4" s="31" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="30" t="s">
-        <v>368</v>
+      <c r="A5" s="31" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="31" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="31" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="31" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="31" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="31" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="31" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="30" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="30" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="30" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="30" t="s">
-        <v>289</v>
-      </c>
-    </row>
     <row r="12">
-      <c r="A12" s="30" t="s">
-        <v>290</v>
+      <c r="A12" s="31" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="30" t="s">
-        <v>369</v>
+      <c r="A13" s="31" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="30" t="s">
-        <v>370</v>
+      <c r="A14" s="31" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="18.25"/>
+    <col customWidth="1" min="2" max="2" width="20.13"/>
+    <col customWidth="1" min="3" max="3" width="19.5"/>
+    <col customWidth="1" min="4" max="4" width="17.38"/>
+    <col customWidth="1" min="5" max="5" width="21.38"/>
+    <col customWidth="1" min="6" max="6" width="26.25"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="21" t="s">
+        <v>374</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>376</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>377</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>378</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="32" t="s">
+        <v>380</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>381</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>382</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>383</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>384</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="32" t="s">
+        <v>386</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>387</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>388</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>389</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>390</v>
+      </c>
+      <c r="F4" s="34" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="32" t="s">
+        <v>391</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>392</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>393</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="E5" s="34" t="s">
+        <v>395</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="32" t="s">
+        <v>397</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>398</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>400</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>401</v>
+      </c>
+      <c r="F6" s="34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>403</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="33" t="s">
+        <v>404</v>
+      </c>
+      <c r="E7" s="34" t="s">
+        <v>405</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="37"/>
+      <c r="B8" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="C8" s="36"/>
+      <c r="D8" s="33" t="s">
+        <v>408</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>409</v>
+      </c>
+      <c r="F8" s="34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="37"/>
+      <c r="B9" s="33" t="s">
+        <v>410</v>
+      </c>
+      <c r="C9" s="36"/>
+      <c r="D9" s="33" t="s">
+        <v>411</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>412</v>
+      </c>
+      <c r="F9" s="38"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="39"/>
+      <c r="B10" s="33" t="s">
+        <v>413</v>
+      </c>
+      <c r="C10" s="36"/>
+      <c r="D10" s="33" t="s">
+        <v>414</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="37"/>
+      <c r="B11" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="40"/>
+      <c r="B12" s="34" t="s">
+        <v>416</v>
+      </c>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="41"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="40"/>
+      <c r="B13" s="34" t="s">
+        <v>417</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="41"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="40"/>
+      <c r="B14" s="34" t="s">
+        <v>418</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="40"/>
+      <c r="B15" s="34" t="s">
+        <v>419</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="40"/>
+      <c r="B16" s="34" t="s">
+        <v>420</v>
+      </c>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="40"/>
+      <c r="B17" s="34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="40"/>
+      <c r="B18" s="34" t="s">
+        <v>422</v>
+      </c>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="40"/>
+      <c r="B19" s="34" t="s">
+        <v>423</v>
+      </c>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="40"/>
+      <c r="B20" s="34" t="s">
+        <v>424</v>
+      </c>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="40"/>
+      <c r="B21" s="34" t="s">
+        <v>425</v>
+      </c>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="40"/>
+      <c r="B22" s="34" t="s">
+        <v>426</v>
+      </c>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="40"/>
+      <c r="B23" s="34" t="s">
+        <v>427</v>
+      </c>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="40"/>
+      <c r="B24" s="34" t="s">
+        <v>428</v>
+      </c>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="40"/>
+      <c r="B25" s="34" t="s">
+        <v>429</v>
+      </c>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="40"/>
+      <c r="B26" s="34" t="s">
+        <v>430</v>
+      </c>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="40"/>
+      <c r="B27" s="34" t="s">
+        <v>431</v>
+      </c>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="40"/>
+      <c r="B28" s="34" t="s">
+        <v>432</v>
+      </c>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="40"/>
+      <c r="B29" s="34" t="s">
+        <v>433</v>
+      </c>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="40"/>
+      <c r="B30" s="34" t="s">
+        <v>434</v>
+      </c>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="40"/>
+      <c r="B31" s="34" t="s">
+        <v>435</v>
+      </c>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="40"/>
+      <c r="B32" s="34" t="s">
+        <v>436</v>
+      </c>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="40"/>
+      <c r="B33" s="34" t="s">
+        <v>437</v>
+      </c>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changes in filter conditions
</commit_message>
<xml_diff>
--- a/src/test/resources/IngredientsAndComorbidities.xlsx
+++ b/src/test/resources/IngredientsAndComorbidities.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="439">
   <si>
     <t>Diabetes</t>
   </si>
@@ -1118,6 +1118,9 @@
   </si>
   <si>
     <t>pea</t>
+  </si>
+  <si>
+    <t>oil</t>
   </si>
   <si>
     <t>Allergies (Bonus points)</t>
@@ -32168,10 +32171,20 @@
       <c r="D92" s="22"/>
     </row>
     <row r="93">
-      <c r="A93" s="22"/>
+      <c r="A93" s="24" t="s">
+        <v>366</v>
+      </c>
       <c r="B93" s="22"/>
       <c r="C93" s="22"/>
       <c r="D93" s="22"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B94" s="22"/>
+      <c r="C94" s="22"/>
+      <c r="D94" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -32196,27 +32209,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="21" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="31" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="31" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="31" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="31" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="6">
@@ -32256,12 +32269,12 @@
     </row>
     <row r="13">
       <c r="A13" s="31" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="31" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -32289,7 +32302,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="19" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -32299,59 +32312,59 @@
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="32" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="F3" s="34" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="32" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="F4" s="34" t="s">
         <v>309</v>
@@ -32359,39 +32372,39 @@
     </row>
     <row r="5">
       <c r="A5" s="32" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="F5" s="34" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="32" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F6" s="34" t="s">
         <v>112</v>
@@ -32399,33 +32412,33 @@
     </row>
     <row r="7">
       <c r="A7" s="32" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C7" s="36"/>
       <c r="D7" s="33" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="F7" s="34" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="37"/>
       <c r="B8" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="33" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="F8" s="34" t="s">
         <v>151</v>
@@ -32434,25 +32447,25 @@
     <row r="9">
       <c r="A9" s="37"/>
       <c r="B9" s="33" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C9" s="36"/>
       <c r="D9" s="33" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F9" s="38"/>
     </row>
     <row r="10">
       <c r="A10" s="39"/>
       <c r="B10" s="33" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C10" s="36"/>
       <c r="D10" s="33" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="E10" s="38"/>
       <c r="F10" s="38"/>
@@ -32460,7 +32473,7 @@
     <row r="11">
       <c r="A11" s="37"/>
       <c r="B11" s="33" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C11" s="36"/>
       <c r="D11" s="36"/>
@@ -32470,7 +32483,7 @@
     <row r="12">
       <c r="A12" s="40"/>
       <c r="B12" s="34" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C12" s="38"/>
       <c r="D12" s="38"/>
@@ -32480,7 +32493,7 @@
     <row r="13">
       <c r="A13" s="40"/>
       <c r="B13" s="34" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
@@ -32490,7 +32503,7 @@
     <row r="14">
       <c r="A14" s="40"/>
       <c r="B14" s="34" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C14" s="38"/>
       <c r="D14" s="38"/>
@@ -32500,7 +32513,7 @@
     <row r="15">
       <c r="A15" s="40"/>
       <c r="B15" s="34" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C15" s="38"/>
       <c r="D15" s="38"/>
@@ -32510,7 +32523,7 @@
     <row r="16">
       <c r="A16" s="40"/>
       <c r="B16" s="34" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C16" s="38"/>
       <c r="D16" s="38"/>
@@ -32520,7 +32533,7 @@
     <row r="17">
       <c r="A17" s="40"/>
       <c r="B17" s="34" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C17" s="38"/>
       <c r="D17" s="38"/>
@@ -32530,7 +32543,7 @@
     <row r="18">
       <c r="A18" s="40"/>
       <c r="B18" s="34" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C18" s="38"/>
       <c r="D18" s="38"/>
@@ -32540,7 +32553,7 @@
     <row r="19">
       <c r="A19" s="40"/>
       <c r="B19" s="34" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C19" s="38"/>
       <c r="D19" s="38"/>
@@ -32550,7 +32563,7 @@
     <row r="20">
       <c r="A20" s="40"/>
       <c r="B20" s="34" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C20" s="38"/>
       <c r="D20" s="38"/>
@@ -32560,7 +32573,7 @@
     <row r="21">
       <c r="A21" s="40"/>
       <c r="B21" s="34" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C21" s="38"/>
       <c r="D21" s="38"/>
@@ -32570,7 +32583,7 @@
     <row r="22">
       <c r="A22" s="40"/>
       <c r="B22" s="34" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
@@ -32580,7 +32593,7 @@
     <row r="23">
       <c r="A23" s="40"/>
       <c r="B23" s="34" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
@@ -32590,7 +32603,7 @@
     <row r="24">
       <c r="A24" s="40"/>
       <c r="B24" s="34" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
@@ -32600,7 +32613,7 @@
     <row r="25">
       <c r="A25" s="40"/>
       <c r="B25" s="34" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C25" s="38"/>
       <c r="D25" s="38"/>
@@ -32610,7 +32623,7 @@
     <row r="26">
       <c r="A26" s="40"/>
       <c r="B26" s="34" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C26" s="38"/>
       <c r="D26" s="38"/>
@@ -32620,7 +32633,7 @@
     <row r="27">
       <c r="A27" s="40"/>
       <c r="B27" s="34" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C27" s="38"/>
       <c r="D27" s="38"/>
@@ -32630,7 +32643,7 @@
     <row r="28">
       <c r="A28" s="40"/>
       <c r="B28" s="34" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C28" s="38"/>
       <c r="D28" s="38"/>
@@ -32640,7 +32653,7 @@
     <row r="29">
       <c r="A29" s="40"/>
       <c r="B29" s="34" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C29" s="38"/>
       <c r="D29" s="38"/>
@@ -32650,7 +32663,7 @@
     <row r="30">
       <c r="A30" s="40"/>
       <c r="B30" s="34" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C30" s="38"/>
       <c r="D30" s="38"/>
@@ -32660,7 +32673,7 @@
     <row r="31">
       <c r="A31" s="40"/>
       <c r="B31" s="34" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C31" s="38"/>
       <c r="D31" s="38"/>
@@ -32670,7 +32683,7 @@
     <row r="32">
       <c r="A32" s="40"/>
       <c r="B32" s="34" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C32" s="38"/>
       <c r="D32" s="38"/>
@@ -32680,7 +32693,7 @@
     <row r="33">
       <c r="A33" s="40"/>
       <c r="B33" s="34" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C33" s="38"/>
       <c r="D33" s="38"/>

</xml_diff>